<commit_message>
[IMP] Import lines from Excel
</commit_message>
<xml_diff>
--- a/account_invoice_import_xlsx/example/example.xlsx
+++ b/account_invoice_import_xlsx/example/example.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Codice</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantità</t>
+    <t xml:space="preserve">Quantita</t>
   </si>
   <si>
     <t xml:space="preserve">Prodotto Alpha</t>
@@ -56,6 +56,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,13 +145,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.96484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>